<commit_message>
New test cases were added
</commit_message>
<xml_diff>
--- a/Swapi/Test cases for Swapi.xlsx
+++ b/Swapi/Test cases for Swapi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Шаги</t>
   </si>
@@ -35,15 +35,9 @@
     <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/                                                Нажать request</t>
   </si>
   <si>
-    <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/ people/3/                                               Нажать request</t>
-  </si>
-  <si>
     <t>Код ответа 200 ОК, json файл с полями name, height, mass, hair_color, skin_color, eye_color, birth_year, gender, homeworld,films, species, vehicles и starships - пустой массив, created, edited, url</t>
   </si>
   <si>
-    <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/ people/13/                                               Нажать request</t>
-  </si>
-  <si>
     <t>Код ответа 200 ОК, json файл с полями как и в предыдущем тест кейсе, только vehicles и starships уже не пустой массив</t>
   </si>
   <si>
@@ -87,6 +81,48 @@
   </si>
   <si>
     <t>Код ответа 200 ОК, json файл с полями people, planets, films, species, vehicles, starships - массивы</t>
+  </si>
+  <si>
+    <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/vehicles/                                               Нажать request</t>
+  </si>
+  <si>
+    <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/people/                                               Нажать request</t>
+  </si>
+  <si>
+    <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/people/13/                                               Нажать request</t>
+  </si>
+  <si>
+    <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/people/3/                                               Нажать request</t>
+  </si>
+  <si>
+    <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/starships/                                               Нажать request</t>
+  </si>
+  <si>
+    <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/films/                                               Нажать request</t>
+  </si>
+  <si>
+    <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/species/                                               Нажать request</t>
+  </si>
+  <si>
+    <t>Зайти на на сайт                                                           Ввести https://swapi.co/api/planets/                                               Нажать request</t>
+  </si>
+  <si>
+    <t>Код ответа 200 ОК, json файл с полями count, next, previous, массив results с информацией о каждом из vehicles; created, edited, url</t>
+  </si>
+  <si>
+    <t>Код ответа 200 ОК, json файл с полями count, next, previous, массив results с информацией о каждом из starships; created, edited, url</t>
+  </si>
+  <si>
+    <t>Код ответа 200 ОК, json файл с полями count, next, previous, массив results с информацией о каждом из people; created, edited, url</t>
+  </si>
+  <si>
+    <t>Код ответа 200 ОК, json файл с полями count, next, previous, массив results с информацией о каждой из planets; created, edited, url</t>
+  </si>
+  <si>
+    <t>Код ответа 200 ОК, json файл с полями count, next, previous, массив results с информацией о каждом из films; created, edited, url</t>
+  </si>
+  <si>
+    <t>Код ответа 200 ОК, json файл с полями count, next, previous, массив results с информацией о каждом из species; created, edited, url</t>
   </si>
 </sst>
 </file>
@@ -440,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,79 +502,127 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>